<commit_message>
último commit como backup
</commit_message>
<xml_diff>
--- a/public/excel/duplicado.xlsx
+++ b/public/excel/duplicado.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="19360" tabRatio="500"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="19360" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Subdivisiones" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>País</t>
   </si>
@@ -113,27 +113,9 @@
     <t>ID789</t>
   </si>
   <si>
-    <t>Universidad Javeriana Sede Bogotá</t>
-  </si>
-  <si>
-    <t>Calle 456 #12-34</t>
-  </si>
-  <si>
-    <t>Jane Doe</t>
-  </si>
-  <si>
-    <t>Rural</t>
-  </si>
-  <si>
-    <t>info.bogota@javeriana.edu.co</t>
-  </si>
-  <si>
     <t>info.cali@javeriana.edu.co</t>
   </si>
   <si>
-    <t>ID098</t>
-  </si>
-  <si>
     <t>Número de documento de identidad</t>
   </si>
   <si>
@@ -141,9 +123,6 @@
   </si>
   <si>
     <t>ID nacional de la sede a la que pertenece</t>
-  </si>
-  <si>
-    <t>Vereda</t>
   </si>
   <si>
     <t>Tipo de primera división</t>
@@ -525,7 +504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -538,13 +517,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -555,7 +534,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -624,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -683,7 +662,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>20</v>
@@ -704,7 +683,7 @@
         <v>1234567890</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>25</v>
@@ -714,39 +693,17 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="3">
-        <v>987654321</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -908,8 +865,6 @@
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1"/>
     <hyperlink ref="J2" r:id="rId2"/>
-    <hyperlink ref="I3" r:id="rId3"/>
-    <hyperlink ref="J3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -917,10 +872,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -932,13 +887,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -950,17 +905,6 @@
       </c>
       <c r="C2" s="3" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="3">
-        <v>987654321</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>